<commit_message>
Added request status tracker feature
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
+++ b/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
@@ -84,7 +84,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
@@ -129,22 +129,16 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
-        <v>46048</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
       <c r="D5">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>46049</v>
+        <v>46048</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -158,7 +152,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>46050</v>
+        <v>46049</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -172,7 +166,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>46051</v>
+        <v>46050</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -186,7 +180,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>46052</v>
+        <v>46051</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -200,7 +194,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>46055</v>
+        <v>46052</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -214,7 +208,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2">
-        <v>46056</v>
+        <v>46055</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
@@ -228,29 +222,43 @@
     </row>
     <row r="12">
       <c r="A12" s="2">
-        <v>46057</v>
+        <v>46056</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
+        <v>46057</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
         <v>46058</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ojt referral form and list front end
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
+++ b/assets/spreadsheets/ojt-001/ojt-001-TIME_SHEET_SUMMARY_.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PhpTrial\assets\spreadsheets\ojt-001\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56218ACA-B73A-419D-81FC-EF487FFEEE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="INTERN_ID" sheetId="1" r:id="rId4"/>
+    <sheet name="INTERN_ID" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
   <si>
     <t>WEEKLY TIME SHEET SUMMARY</t>
   </si>
@@ -104,34 +109,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
+      <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -186,22 +180,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -525,26 +527,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A10">
-      <selection activeCell="A1" sqref="A1:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.139" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="15.139" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="17.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="29.279" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" customHeight="1" ht="21">
+    <row r="1" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -553,14 +552,14 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:5" customHeight="1" ht="15">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" customHeight="1" ht="15.75">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -577,7 +576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -594,7 +593,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -611,7 +610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -628,7 +627,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -645,7 +644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -662,7 +661,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -679,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -696,7 +695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -713,7 +712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -730,7 +729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -747,7 +746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -764,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -781,7 +780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -798,7 +797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -809,13 +808,13 @@
         <v>8</v>
       </c>
       <c r="D17" s="2">
-        <v>8.38</v>
+        <v>8.3800000000000008</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -826,18 +825,16 @@
         <v>8</v>
       </c>
       <c r="D18" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="1">
     <mergeCell ref="A1:E2"/>
   </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
 </worksheet>
 </file>
</xml_diff>